<commit_message>
Added headings in excel
</commit_message>
<xml_diff>
--- a/Rules.xlsx
+++ b/Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rsrko\Documents\UiPath\Assignment 4 Email Categorisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97045554-CF76-4ED3-B7EE-4AA3A689A75C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA4B423-979C-4C3B-BCF1-D08E4FDF8DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="228" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Important</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>with love</t>
+  </si>
+  <si>
+    <t>Folder Name</t>
+  </si>
+  <si>
+    <t>Keyword</t>
   </si>
 </sst>
 </file>
@@ -354,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -367,17 +373,25 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>